<commit_message>
Changed efficiency column name from "eta" to "Lighting Efficiency [%]"
</commit_message>
<xml_diff>
--- a/Data/SEA_lighting_efficiency.xlsx
+++ b/Data/SEA_lighting_efficiency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDE60DE1-0F09-4E07-A84A-A2420D492B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEAA570-2E36-4D13-8924-4D30566645DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{841F0BE4-586F-4133-96F7-704F58268F03}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Eta</t>
-  </si>
-  <si>
     <t>China</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Lighting Efficiency [%]</t>
   </si>
 </sst>
 </file>
@@ -2159,6 +2159,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -2169,12 +2170,12 @@
         <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1">
         <v>1960</v>
@@ -2185,7 +2186,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>1961</v>
@@ -2196,7 +2197,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
         <v>1962</v>
@@ -2207,7 +2208,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1">
         <v>1963</v>
@@ -2218,7 +2219,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>1964</v>
@@ -2229,7 +2230,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>1965</v>
@@ -2240,7 +2241,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1">
         <v>1966</v>
@@ -2251,7 +2252,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>1967</v>
@@ -2262,7 +2263,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1">
         <v>1968</v>
@@ -2273,7 +2274,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1">
         <v>1969</v>
@@ -2284,7 +2285,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>1970</v>
@@ -2295,7 +2296,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1">
         <v>1971</v>
@@ -2306,7 +2307,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1">
         <v>1972</v>
@@ -2317,7 +2318,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1">
         <v>1973</v>
@@ -2328,7 +2329,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1">
         <v>1974</v>
@@ -2339,7 +2340,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>1975</v>
@@ -2350,7 +2351,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1">
         <v>1976</v>
@@ -2361,7 +2362,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1">
         <v>1977</v>
@@ -2372,7 +2373,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>1978</v>
@@ -2383,7 +2384,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
         <v>1979</v>
@@ -2394,7 +2395,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1">
         <v>1980</v>
@@ -2405,7 +2406,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1">
         <v>1981</v>
@@ -2416,7 +2417,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
         <v>1982</v>
@@ -2427,7 +2428,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>1983</v>
@@ -2438,7 +2439,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1">
         <v>1984</v>
@@ -2449,7 +2450,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1">
         <v>1985</v>
@@ -2460,7 +2461,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1">
         <v>1986</v>
@@ -2471,7 +2472,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="1">
         <v>1987</v>
@@ -2482,7 +2483,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1">
         <v>1988</v>
@@ -2493,7 +2494,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1">
         <v>1989</v>
@@ -2504,7 +2505,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1">
         <v>1990</v>
@@ -2515,7 +2516,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1">
         <v>1991</v>
@@ -2526,7 +2527,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1">
         <v>1992</v>
@@ -2537,7 +2538,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" s="1">
         <v>1993</v>
@@ -2548,7 +2549,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="1">
         <v>1994</v>
@@ -2559,7 +2560,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" s="1">
         <v>1995</v>
@@ -2570,7 +2571,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="1">
         <v>1996</v>
@@ -2581,7 +2582,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" s="1">
         <v>1997</v>
@@ -2592,7 +2593,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" s="1">
         <v>1998</v>
@@ -2603,7 +2604,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B41" s="1">
         <v>1999</v>
@@ -2614,7 +2615,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" s="1">
         <v>2000</v>
@@ -2625,7 +2626,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" s="1">
         <v>2001</v>
@@ -2636,7 +2637,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" s="1">
         <v>2002</v>
@@ -2647,7 +2648,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45" s="1">
         <v>2003</v>
@@ -2658,7 +2659,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B46" s="1">
         <v>2004</v>
@@ -2669,7 +2670,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B47" s="1">
         <v>2005</v>
@@ -2680,7 +2681,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" s="1">
         <v>2006</v>
@@ -2691,7 +2692,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B49" s="1">
         <v>2007</v>
@@ -2702,7 +2703,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="1">
         <v>2008</v>
@@ -2713,7 +2714,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51" s="1">
         <v>2009</v>
@@ -2724,7 +2725,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" s="1">
         <v>2010</v>
@@ -2735,7 +2736,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" s="1">
         <v>2011</v>
@@ -2746,7 +2747,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B54" s="1">
         <v>2012</v>
@@ -2757,7 +2758,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" s="1">
         <v>2013</v>
@@ -2768,7 +2769,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B56" s="1">
         <v>2014</v>
@@ -2779,7 +2780,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B57" s="1">
         <v>2015</v>
@@ -2790,7 +2791,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B58" s="1">
         <v>2016</v>
@@ -2801,7 +2802,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" s="1">
         <v>2017</v>
@@ -2812,7 +2813,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B60" s="1">
         <v>1960</v>
@@ -2823,7 +2824,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B61" s="1">
         <v>1961</v>
@@ -2834,7 +2835,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B62" s="1">
         <v>1962</v>
@@ -2845,7 +2846,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B63" s="1">
         <v>1963</v>
@@ -2856,7 +2857,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B64" s="1">
         <v>1964</v>
@@ -2867,7 +2868,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B65" s="1">
         <v>1965</v>
@@ -2878,7 +2879,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B66" s="1">
         <v>1966</v>
@@ -2889,7 +2890,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B67" s="1">
         <v>1967</v>
@@ -2900,7 +2901,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B68" s="1">
         <v>1968</v>
@@ -2911,7 +2912,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B69" s="1">
         <v>1969</v>
@@ -2922,7 +2923,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B70" s="1">
         <v>1970</v>
@@ -2933,7 +2934,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B71" s="1">
         <v>1971</v>
@@ -2944,7 +2945,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B72" s="1">
         <v>1972</v>
@@ -2955,7 +2956,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B73" s="1">
         <v>1973</v>
@@ -2966,7 +2967,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B74" s="1">
         <v>1974</v>
@@ -2977,7 +2978,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B75" s="1">
         <v>1975</v>
@@ -2988,7 +2989,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B76" s="1">
         <v>1976</v>
@@ -2999,7 +3000,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B77" s="1">
         <v>1977</v>
@@ -3010,7 +3011,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B78" s="1">
         <v>1978</v>
@@ -3021,7 +3022,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B79" s="1">
         <v>1979</v>
@@ -3032,7 +3033,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B80" s="1">
         <v>1980</v>
@@ -3043,7 +3044,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B81" s="1">
         <v>1981</v>
@@ -3054,7 +3055,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B82" s="1">
         <v>1982</v>
@@ -3065,7 +3066,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B83" s="1">
         <v>1983</v>
@@ -3076,7 +3077,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B84" s="1">
         <v>1984</v>
@@ -3087,7 +3088,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B85" s="1">
         <v>1985</v>
@@ -3098,7 +3099,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B86" s="1">
         <v>1986</v>
@@ -3109,7 +3110,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B87" s="1">
         <v>1987</v>
@@ -3120,7 +3121,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B88" s="1">
         <v>1988</v>
@@ -3131,7 +3132,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B89" s="1">
         <v>1989</v>
@@ -3142,7 +3143,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B90" s="1">
         <v>1990</v>
@@ -3153,7 +3154,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B91" s="1">
         <v>1991</v>
@@ -3164,7 +3165,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B92" s="1">
         <v>1992</v>
@@ -3175,7 +3176,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B93" s="1">
         <v>1993</v>
@@ -3186,7 +3187,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B94" s="1">
         <v>1994</v>
@@ -3197,7 +3198,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B95" s="1">
         <v>1995</v>
@@ -3208,7 +3209,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B96" s="1">
         <v>1996</v>
@@ -3219,7 +3220,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B97" s="1">
         <v>1997</v>
@@ -3230,7 +3231,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B98" s="1">
         <v>1998</v>
@@ -3241,7 +3242,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B99" s="1">
         <v>1999</v>
@@ -3252,7 +3253,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B100" s="1">
         <v>2000</v>
@@ -3263,7 +3264,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B101" s="1">
         <v>2001</v>
@@ -3274,7 +3275,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B102" s="1">
         <v>2002</v>
@@ -3285,7 +3286,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B103" s="1">
         <v>2003</v>
@@ -3296,7 +3297,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B104" s="1">
         <v>2004</v>
@@ -3307,7 +3308,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B105" s="1">
         <v>2005</v>
@@ -3318,7 +3319,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B106" s="1">
         <v>2006</v>
@@ -3329,7 +3330,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B107" s="1">
         <v>2007</v>
@@ -3340,7 +3341,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B108" s="1">
         <v>2008</v>
@@ -3351,7 +3352,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B109" s="1">
         <v>2009</v>
@@ -3362,7 +3363,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B110" s="1">
         <v>2010</v>
@@ -3373,7 +3374,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B111" s="1">
         <v>2011</v>
@@ -3384,7 +3385,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B112" s="1">
         <v>2012</v>
@@ -3395,7 +3396,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B113" s="1">
         <v>2013</v>
@@ -3406,7 +3407,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B114" s="1">
         <v>2014</v>
@@ -3417,7 +3418,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B115" s="1">
         <v>2015</v>
@@ -3428,7 +3429,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B116" s="1">
         <v>2016</v>
@@ -3439,7 +3440,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B117" s="1">
         <v>2017</v>
@@ -3450,7 +3451,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B118" s="1">
         <v>1960</v>
@@ -3461,7 +3462,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B119" s="1">
         <v>1961</v>
@@ -3472,7 +3473,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B120" s="1">
         <v>1962</v>
@@ -3483,7 +3484,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B121" s="1">
         <v>1963</v>
@@ -3494,7 +3495,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B122" s="1">
         <v>1964</v>
@@ -3505,7 +3506,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B123" s="1">
         <v>1965</v>
@@ -3516,7 +3517,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B124" s="1">
         <v>1966</v>
@@ -3527,7 +3528,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B125" s="1">
         <v>1967</v>
@@ -3538,7 +3539,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B126" s="1">
         <v>1968</v>
@@ -3549,7 +3550,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B127" s="1">
         <v>1969</v>
@@ -3560,7 +3561,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B128" s="1">
         <v>1970</v>
@@ -3571,7 +3572,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B129" s="1">
         <v>1971</v>
@@ -3582,7 +3583,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B130" s="1">
         <v>1972</v>
@@ -3593,7 +3594,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B131" s="1">
         <v>1973</v>
@@ -3604,7 +3605,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B132" s="1">
         <v>1974</v>
@@ -3615,7 +3616,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B133" s="1">
         <v>1975</v>
@@ -3626,7 +3627,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B134" s="1">
         <v>1976</v>
@@ -3637,7 +3638,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B135" s="1">
         <v>1977</v>
@@ -3648,7 +3649,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B136" s="1">
         <v>1978</v>
@@ -3659,7 +3660,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B137" s="1">
         <v>1979</v>
@@ -3670,7 +3671,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B138" s="1">
         <v>1980</v>
@@ -3681,7 +3682,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B139" s="1">
         <v>1981</v>
@@ -3692,7 +3693,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B140" s="1">
         <v>1982</v>
@@ -3703,7 +3704,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B141" s="1">
         <v>1983</v>
@@ -3714,7 +3715,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B142" s="1">
         <v>1984</v>
@@ -3725,7 +3726,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B143" s="1">
         <v>1985</v>
@@ -3736,7 +3737,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B144" s="1">
         <v>1986</v>
@@ -3747,7 +3748,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B145" s="1">
         <v>1987</v>
@@ -3758,7 +3759,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B146" s="1">
         <v>1988</v>
@@ -3769,7 +3770,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B147" s="1">
         <v>1989</v>
@@ -3780,7 +3781,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B148" s="1">
         <v>1990</v>
@@ -3791,7 +3792,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B149" s="1">
         <v>1991</v>
@@ -3802,7 +3803,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B150" s="1">
         <v>1992</v>
@@ -3813,7 +3814,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B151" s="1">
         <v>1993</v>
@@ -3824,7 +3825,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B152" s="1">
         <v>1994</v>
@@ -3835,7 +3836,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B153" s="1">
         <v>1995</v>
@@ -3846,7 +3847,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B154" s="1">
         <v>1996</v>
@@ -3857,7 +3858,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B155" s="1">
         <v>1997</v>
@@ -3868,7 +3869,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B156" s="1">
         <v>1998</v>
@@ -3879,7 +3880,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B157" s="1">
         <v>1999</v>
@@ -3890,7 +3891,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B158" s="1">
         <v>2000</v>
@@ -3901,7 +3902,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B159" s="1">
         <v>2001</v>
@@ -3912,7 +3913,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B160" s="1">
         <v>2002</v>
@@ -3923,7 +3924,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B161" s="1">
         <v>2003</v>
@@ -3934,7 +3935,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B162" s="1">
         <v>2004</v>
@@ -3945,7 +3946,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B163" s="1">
         <v>2005</v>
@@ -3956,7 +3957,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B164" s="1">
         <v>2006</v>
@@ -3967,7 +3968,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B165" s="1">
         <v>2007</v>
@@ -3978,7 +3979,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B166" s="1">
         <v>2008</v>
@@ -3989,7 +3990,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B167" s="1">
         <v>2009</v>
@@ -4000,7 +4001,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B168" s="1">
         <v>2010</v>
@@ -4011,7 +4012,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B169" s="1">
         <v>2011</v>
@@ -4022,7 +4023,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B170" s="1">
         <v>2012</v>
@@ -4033,7 +4034,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B171" s="1">
         <v>2013</v>
@@ -4044,7 +4045,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B172" s="1">
         <v>2014</v>
@@ -4055,7 +4056,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B173" s="1">
         <v>2015</v>
@@ -4066,7 +4067,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B174" s="1">
         <v>2016</v>
@@ -4077,7 +4078,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B175" s="1">
         <v>2017</v>
@@ -4088,7 +4089,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B176" s="1">
         <v>1960</v>
@@ -4099,7 +4100,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B177" s="1">
         <v>1961</v>
@@ -4110,7 +4111,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B178" s="1">
         <v>1962</v>
@@ -4121,7 +4122,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B179" s="1">
         <v>1963</v>
@@ -4132,7 +4133,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B180" s="1">
         <v>1964</v>
@@ -4143,7 +4144,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B181" s="1">
         <v>1965</v>
@@ -4154,7 +4155,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B182" s="1">
         <v>1966</v>
@@ -4165,7 +4166,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B183" s="1">
         <v>1967</v>
@@ -4176,7 +4177,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B184" s="1">
         <v>1968</v>
@@ -4187,7 +4188,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B185" s="1">
         <v>1969</v>
@@ -4198,7 +4199,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B186" s="1">
         <v>1970</v>
@@ -4209,7 +4210,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B187" s="1">
         <v>1971</v>
@@ -4220,7 +4221,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B188" s="1">
         <v>1972</v>
@@ -4231,7 +4232,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B189" s="1">
         <v>1973</v>
@@ -4242,7 +4243,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B190" s="1">
         <v>1974</v>
@@ -4253,7 +4254,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B191" s="1">
         <v>1975</v>
@@ -4264,7 +4265,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B192" s="1">
         <v>1976</v>
@@ -4275,7 +4276,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B193" s="1">
         <v>1977</v>
@@ -4286,7 +4287,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B194" s="1">
         <v>1978</v>
@@ -4297,7 +4298,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B195" s="1">
         <v>1979</v>
@@ -4308,7 +4309,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B196" s="1">
         <v>1980</v>
@@ -4319,7 +4320,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B197" s="1">
         <v>1981</v>
@@ -4330,7 +4331,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B198" s="1">
         <v>1982</v>
@@ -4341,7 +4342,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B199" s="1">
         <v>1983</v>
@@ -4352,7 +4353,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B200" s="1">
         <v>1984</v>
@@ -4363,7 +4364,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B201" s="1">
         <v>1985</v>
@@ -4374,7 +4375,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B202" s="1">
         <v>1986</v>
@@ -4385,7 +4386,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B203" s="1">
         <v>1987</v>
@@ -4396,7 +4397,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B204" s="1">
         <v>1988</v>
@@ -4407,7 +4408,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B205" s="1">
         <v>1989</v>
@@ -4418,7 +4419,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B206" s="1">
         <v>1990</v>
@@ -4429,7 +4430,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B207" s="1">
         <v>1991</v>
@@ -4440,7 +4441,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B208" s="1">
         <v>1992</v>
@@ -4451,7 +4452,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B209" s="1">
         <v>1993</v>
@@ -4462,7 +4463,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B210" s="1">
         <v>1994</v>
@@ -4473,7 +4474,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B211" s="1">
         <v>1995</v>
@@ -4484,7 +4485,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B212" s="1">
         <v>1996</v>
@@ -4495,7 +4496,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B213" s="1">
         <v>1997</v>
@@ -4506,7 +4507,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B214" s="1">
         <v>1998</v>
@@ -4517,7 +4518,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B215" s="1">
         <v>1999</v>
@@ -4528,7 +4529,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B216" s="1">
         <v>2000</v>
@@ -4539,7 +4540,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B217" s="1">
         <v>2001</v>
@@ -4550,7 +4551,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B218" s="1">
         <v>2002</v>
@@ -4561,7 +4562,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B219" s="1">
         <v>2003</v>
@@ -4572,7 +4573,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B220" s="1">
         <v>2004</v>
@@ -4583,7 +4584,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B221" s="1">
         <v>2005</v>
@@ -4594,7 +4595,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B222" s="1">
         <v>2006</v>
@@ -4605,7 +4606,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B223" s="1">
         <v>2007</v>
@@ -4616,7 +4617,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B224" s="1">
         <v>2008</v>
@@ -4627,7 +4628,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B225" s="1">
         <v>2009</v>
@@ -4638,7 +4639,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B226" s="1">
         <v>2010</v>
@@ -4649,7 +4650,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B227" s="1">
         <v>2011</v>
@@ -4660,7 +4661,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B228" s="1">
         <v>2012</v>
@@ -4671,7 +4672,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B229" s="1">
         <v>2013</v>
@@ -4682,7 +4683,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B230" s="1">
         <v>2014</v>
@@ -4693,7 +4694,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B231" s="1">
         <v>2015</v>
@@ -4704,7 +4705,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B232" s="1">
         <v>2016</v>
@@ -4715,7 +4716,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B233" s="1">
         <v>2017</v>
@@ -4726,7 +4727,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B234" s="1">
         <v>1960</v>
@@ -4737,7 +4738,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B235" s="1">
         <v>1961</v>
@@ -4748,7 +4749,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B236" s="1">
         <v>1962</v>
@@ -4759,7 +4760,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B237" s="1">
         <v>1963</v>
@@ -4770,7 +4771,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B238" s="1">
         <v>1964</v>
@@ -4781,7 +4782,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B239" s="1">
         <v>1965</v>
@@ -4792,7 +4793,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B240" s="1">
         <v>1966</v>
@@ -4803,7 +4804,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B241" s="1">
         <v>1967</v>
@@ -4814,7 +4815,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B242" s="1">
         <v>1968</v>
@@ -4825,7 +4826,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B243" s="1">
         <v>1969</v>
@@ -4836,7 +4837,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B244" s="1">
         <v>1970</v>
@@ -4847,7 +4848,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B245" s="1">
         <v>1971</v>
@@ -4858,7 +4859,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B246" s="1">
         <v>1972</v>
@@ -4869,7 +4870,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B247" s="1">
         <v>1973</v>
@@ -4880,7 +4881,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B248" s="1">
         <v>1974</v>
@@ -4891,7 +4892,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B249" s="1">
         <v>1975</v>
@@ -4902,7 +4903,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B250" s="1">
         <v>1976</v>
@@ -4913,7 +4914,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B251" s="1">
         <v>1977</v>
@@ -4924,7 +4925,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B252" s="1">
         <v>1978</v>
@@ -4935,7 +4936,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B253" s="1">
         <v>1979</v>
@@ -4946,7 +4947,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B254" s="1">
         <v>1980</v>
@@ -4957,7 +4958,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B255" s="1">
         <v>1981</v>
@@ -4968,7 +4969,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B256" s="1">
         <v>1982</v>
@@ -4979,7 +4980,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B257" s="1">
         <v>1983</v>
@@ -4990,7 +4991,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B258" s="1">
         <v>1984</v>
@@ -5001,7 +5002,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B259" s="1">
         <v>1985</v>
@@ -5012,7 +5013,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B260" s="1">
         <v>1986</v>
@@ -5023,7 +5024,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B261" s="1">
         <v>1987</v>
@@ -5034,7 +5035,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B262" s="1">
         <v>1988</v>
@@ -5045,7 +5046,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B263" s="1">
         <v>1989</v>
@@ -5056,7 +5057,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B264" s="1">
         <v>1990</v>
@@ -5067,7 +5068,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B265" s="1">
         <v>1991</v>
@@ -5078,7 +5079,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B266" s="1">
         <v>1992</v>
@@ -5089,7 +5090,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B267" s="1">
         <v>1993</v>
@@ -5100,7 +5101,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B268" s="1">
         <v>1994</v>
@@ -5111,7 +5112,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B269" s="1">
         <v>1995</v>
@@ -5122,7 +5123,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B270" s="1">
         <v>1996</v>
@@ -5133,7 +5134,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B271" s="1">
         <v>1997</v>
@@ -5144,7 +5145,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B272" s="1">
         <v>1998</v>
@@ -5155,7 +5156,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B273" s="1">
         <v>1999</v>
@@ -5166,7 +5167,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B274" s="1">
         <v>2000</v>
@@ -5177,7 +5178,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B275" s="1">
         <v>2001</v>
@@ -5188,7 +5189,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B276" s="1">
         <v>2002</v>
@@ -5199,7 +5200,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B277" s="1">
         <v>2003</v>
@@ -5210,7 +5211,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B278" s="1">
         <v>2004</v>
@@ -5221,7 +5222,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B279" s="1">
         <v>2005</v>
@@ -5232,7 +5233,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B280" s="1">
         <v>2006</v>
@@ -5243,7 +5244,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B281" s="1">
         <v>2007</v>
@@ -5254,7 +5255,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B282" s="1">
         <v>2008</v>
@@ -5265,7 +5266,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B283" s="1">
         <v>2009</v>
@@ -5276,7 +5277,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B284" s="1">
         <v>2010</v>
@@ -5287,7 +5288,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B285" s="1">
         <v>2011</v>
@@ -5298,7 +5299,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B286" s="1">
         <v>2012</v>
@@ -5309,7 +5310,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B287" s="1">
         <v>2013</v>
@@ -5320,7 +5321,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B288" s="1">
         <v>2014</v>
@@ -5331,7 +5332,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B289" s="1">
         <v>2015</v>
@@ -5342,7 +5343,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B290" s="1">
         <v>2016</v>
@@ -5353,7 +5354,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B291" s="1">
         <v>2017</v>
@@ -5364,7 +5365,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B292" s="1">
         <v>1960</v>
@@ -5375,7 +5376,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B293" s="1">
         <v>1961</v>
@@ -5386,7 +5387,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B294" s="1">
         <v>1962</v>
@@ -5397,7 +5398,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B295" s="1">
         <v>1963</v>
@@ -5408,7 +5409,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B296" s="1">
         <v>1964</v>
@@ -5419,7 +5420,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B297" s="1">
         <v>1965</v>
@@ -5430,7 +5431,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B298" s="1">
         <v>1966</v>
@@ -5441,7 +5442,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B299" s="1">
         <v>1967</v>
@@ -5452,7 +5453,7 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B300" s="1">
         <v>1968</v>
@@ -5463,7 +5464,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B301" s="1">
         <v>1969</v>
@@ -5474,7 +5475,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B302" s="1">
         <v>1970</v>
@@ -5485,7 +5486,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B303" s="1">
         <v>1971</v>
@@ -5496,7 +5497,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B304" s="1">
         <v>1972</v>
@@ -5507,7 +5508,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B305" s="1">
         <v>1973</v>
@@ -5518,7 +5519,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B306" s="1">
         <v>1974</v>
@@ -5529,7 +5530,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B307" s="1">
         <v>1975</v>
@@ -5540,7 +5541,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B308" s="1">
         <v>1976</v>
@@ -5551,7 +5552,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B309" s="1">
         <v>1977</v>
@@ -5562,7 +5563,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B310" s="1">
         <v>1978</v>
@@ -5573,7 +5574,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B311" s="1">
         <v>1979</v>
@@ -5584,7 +5585,7 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B312" s="1">
         <v>1980</v>
@@ -5595,7 +5596,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B313" s="1">
         <v>1981</v>
@@ -5606,7 +5607,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B314" s="1">
         <v>1982</v>
@@ -5617,7 +5618,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B315" s="1">
         <v>1983</v>
@@ -5628,7 +5629,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B316" s="1">
         <v>1984</v>
@@ -5639,7 +5640,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B317" s="1">
         <v>1985</v>
@@ -5650,7 +5651,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B318" s="1">
         <v>1986</v>
@@ -5661,7 +5662,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B319" s="1">
         <v>1987</v>
@@ -5672,7 +5673,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B320" s="1">
         <v>1988</v>
@@ -5683,7 +5684,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B321" s="1">
         <v>1989</v>
@@ -5694,7 +5695,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B322" s="1">
         <v>1990</v>
@@ -5705,7 +5706,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B323" s="1">
         <v>1991</v>
@@ -5716,7 +5717,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B324" s="1">
         <v>1992</v>
@@ -5727,7 +5728,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B325" s="1">
         <v>1993</v>
@@ -5738,7 +5739,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B326" s="1">
         <v>1994</v>
@@ -5749,7 +5750,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B327" s="1">
         <v>1995</v>
@@ -5760,7 +5761,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B328" s="1">
         <v>1996</v>
@@ -5771,7 +5772,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B329" s="1">
         <v>1997</v>
@@ -5782,7 +5783,7 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B330" s="1">
         <v>1998</v>
@@ -5793,7 +5794,7 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B331" s="1">
         <v>1999</v>
@@ -5804,7 +5805,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B332" s="1">
         <v>2000</v>
@@ -5815,7 +5816,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B333" s="1">
         <v>2001</v>
@@ -5826,7 +5827,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B334" s="1">
         <v>2002</v>
@@ -5837,7 +5838,7 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B335" s="1">
         <v>2003</v>
@@ -5848,7 +5849,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B336" s="1">
         <v>2004</v>
@@ -5859,7 +5860,7 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B337" s="1">
         <v>2005</v>
@@ -5870,7 +5871,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B338" s="1">
         <v>2006</v>
@@ -5881,7 +5882,7 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B339" s="1">
         <v>2007</v>
@@ -5892,7 +5893,7 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B340" s="1">
         <v>2008</v>
@@ -5903,7 +5904,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B341" s="1">
         <v>2009</v>
@@ -5914,7 +5915,7 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B342" s="1">
         <v>2010</v>
@@ -5925,7 +5926,7 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B343" s="1">
         <v>2011</v>
@@ -5936,7 +5937,7 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B344" s="1">
         <v>2012</v>
@@ -5947,7 +5948,7 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B345" s="1">
         <v>2013</v>
@@ -5958,7 +5959,7 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B346" s="1">
         <v>2014</v>
@@ -5969,7 +5970,7 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B347" s="1">
         <v>2015</v>
@@ -5980,7 +5981,7 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B348" s="1">
         <v>2016</v>
@@ -5991,7 +5992,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B349" s="1">
         <v>2017</v>
@@ -6002,7 +6003,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B350" s="1">
         <v>1960</v>
@@ -6010,7 +6011,7 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B351" s="1">
         <v>1961</v>
@@ -6018,7 +6019,7 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B352" s="1">
         <v>1962</v>
@@ -6026,7 +6027,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B353" s="1">
         <v>1963</v>
@@ -6034,7 +6035,7 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B354" s="1">
         <v>1964</v>
@@ -6042,7 +6043,7 @@
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B355" s="1">
         <v>1965</v>
@@ -6050,7 +6051,7 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B356" s="1">
         <v>1966</v>
@@ -6058,7 +6059,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B357" s="1">
         <v>1967</v>
@@ -6066,7 +6067,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B358" s="1">
         <v>1968</v>
@@ -6074,7 +6075,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B359" s="1">
         <v>1969</v>
@@ -6082,7 +6083,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B360" s="1">
         <v>1970</v>
@@ -6090,7 +6091,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B361" s="1">
         <v>1971</v>
@@ -6098,7 +6099,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B362" s="1">
         <v>1972</v>
@@ -6106,7 +6107,7 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B363" s="1">
         <v>1973</v>
@@ -6114,7 +6115,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B364" s="1">
         <v>1974</v>
@@ -6122,7 +6123,7 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B365" s="1">
         <v>1975</v>
@@ -6130,7 +6131,7 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B366" s="1">
         <v>1976</v>
@@ -6138,7 +6139,7 @@
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B367" s="1">
         <v>1977</v>
@@ -6146,7 +6147,7 @@
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B368" s="1">
         <v>1978</v>
@@ -6154,7 +6155,7 @@
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B369" s="1">
         <v>1979</v>
@@ -6162,7 +6163,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B370" s="1">
         <v>1980</v>
@@ -6170,7 +6171,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B371" s="1">
         <v>1981</v>
@@ -6178,7 +6179,7 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B372" s="1">
         <v>1982</v>
@@ -6186,7 +6187,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B373" s="1">
         <v>1983</v>
@@ -6194,7 +6195,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B374" s="1">
         <v>1984</v>
@@ -6202,7 +6203,7 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B375" s="1">
         <v>1985</v>
@@ -6210,7 +6211,7 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B376" s="1">
         <v>1986</v>
@@ -6218,7 +6219,7 @@
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B377" s="1">
         <v>1987</v>
@@ -6226,7 +6227,7 @@
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B378" s="1">
         <v>1988</v>
@@ -6234,7 +6235,7 @@
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B379" s="1">
         <v>1989</v>
@@ -6242,7 +6243,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B380" s="1">
         <v>1990</v>
@@ -6250,7 +6251,7 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B381" s="1">
         <v>1991</v>
@@ -6258,7 +6259,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B382" s="1">
         <v>1992</v>
@@ -6266,7 +6267,7 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B383" s="1">
         <v>1993</v>
@@ -6274,7 +6275,7 @@
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B384" s="1">
         <v>1994</v>
@@ -6282,7 +6283,7 @@
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B385" s="1">
         <v>1995</v>
@@ -6290,7 +6291,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B386" s="1">
         <v>1996</v>
@@ -6298,7 +6299,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B387" s="1">
         <v>1997</v>
@@ -6306,7 +6307,7 @@
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B388" s="1">
         <v>1998</v>
@@ -6314,7 +6315,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B389" s="1">
         <v>1999</v>
@@ -6322,7 +6323,7 @@
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B390" s="1">
         <v>2000</v>
@@ -6330,7 +6331,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B391" s="1">
         <v>2001</v>
@@ -6338,7 +6339,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B392" s="1">
         <v>2002</v>
@@ -6346,7 +6347,7 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B393" s="1">
         <v>2003</v>
@@ -6354,7 +6355,7 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B394" s="1">
         <v>2004</v>
@@ -6362,7 +6363,7 @@
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B395" s="1">
         <v>2005</v>
@@ -6370,7 +6371,7 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B396" s="1">
         <v>2006</v>
@@ -6378,7 +6379,7 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B397" s="1">
         <v>2007</v>
@@ -6386,7 +6387,7 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B398" s="1">
         <v>2008</v>
@@ -6394,7 +6395,7 @@
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B399" s="1">
         <v>2009</v>
@@ -6402,7 +6403,7 @@
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B400" s="1">
         <v>2010</v>
@@ -6410,7 +6411,7 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B401" s="1">
         <v>2011</v>
@@ -6418,7 +6419,7 @@
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B402" s="1">
         <v>2012</v>
@@ -6426,7 +6427,7 @@
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B403" s="1">
         <v>2013</v>
@@ -6434,7 +6435,7 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B404" s="1">
         <v>2014</v>
@@ -6442,7 +6443,7 @@
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B405" s="1">
         <v>2015</v>
@@ -6450,7 +6451,7 @@
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B406" s="1">
         <v>2016</v>
@@ -6458,7 +6459,7 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B407" s="1">
         <v>2017</v>

</xml_diff>